<commit_message>
added opmerking to backlog
</commit_message>
<xml_diff>
--- a/planning/Backlog.xlsx
+++ b/planning/Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djord\Desktop\hz\1rd-GameDev\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{56E5421D-9F4A-45AA-9FE0-0F819DD864ED}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC72F50-D174-49A9-94BE-F340F1443E82}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" xr2:uid="{5F1A6B09-E755-4ACD-9711-4797947383CE}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="35">
   <si>
     <t>ROL:</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Progressie bewaren</t>
   </si>
   <si>
-    <t>Building selecteren</t>
-  </si>
-  <si>
     <t>om te kunnen bouwen</t>
   </si>
   <si>
@@ -94,6 +91,45 @@
   </si>
   <si>
     <t>uniekheid</t>
+  </si>
+  <si>
+    <t>Building selecteren en neerzetten</t>
+  </si>
+  <si>
+    <t>Building upgrades</t>
+  </si>
+  <si>
+    <t>groter/sneller/beter verdienend maken</t>
+  </si>
+  <si>
+    <t>3 huizen bij elkaar wordt een dorp, etc</t>
+  </si>
+  <si>
+    <t>meer geld verdienen en grotere populatie krijgen</t>
+  </si>
+  <si>
+    <t>populatie counter</t>
+  </si>
+  <si>
+    <t>kunnen zien hoe groot/snel je populatie groeit</t>
+  </si>
+  <si>
+    <t>Markt die random verschijnt op de map,</t>
+  </si>
+  <si>
+    <t>Goedkopere resources, snellere progressie</t>
+  </si>
+  <si>
+    <t>Natuurvervuiling visueel laten zien</t>
+  </si>
+  <si>
+    <t>laat duidelijk gevolgen zien, ziet er mooier uit</t>
+  </si>
+  <si>
+    <t>Krijg geld van bomen kappen</t>
+  </si>
+  <si>
+    <t>krijg geld als je geen inkomen hebt</t>
   </si>
 </sst>
 </file>
@@ -135,27 +171,7 @@
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color theme="4"/>
@@ -168,16 +184,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -501,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0FF629C-D8EC-48FB-97D4-BA4C759AD122}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -541,10 +547,10 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -564,7 +570,7 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -578,13 +584,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -598,13 +604,13 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -618,13 +624,13 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
         <v>17</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>18</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -638,30 +644,150 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
         <v>21</v>
       </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
       <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
         <v>15</v>
       </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",F1)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="In progress">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="In progress">
       <formula>NOT(ISERROR(SEARCH("In progress",F1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>